<commit_message>
add cheque pending search
</commit_message>
<xml_diff>
--- a/src/main/resources/Financial_Report.xlsx
+++ b/src/main/resources/Financial_Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Works\projects\church-app\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F4101F3-8F1A-466C-B3BC-519FD503014D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C7BC755-8F32-42D2-BA70-599AEF986FB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="-110" windowWidth="18490" windowHeight="11020" xr2:uid="{7F8DEBD6-32E0-4BF8-87C4-D1C13E633F04}"/>
+    <workbookView xWindow="820" yWindow="-110" windowWidth="18490" windowHeight="11020" activeTab="1" xr2:uid="{7F8DEBD6-32E0-4BF8-87C4-D1C13E633F04}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -794,9 +794,6 @@
     <t>교인주소록</t>
   </si>
   <si>
-    <t>New Horizons for Seniors Program</t>
-  </si>
-  <si>
     <t>05-7515-022</t>
   </si>
   <si>
@@ -834,6 +831,9 @@
   </si>
   <si>
     <t>'23 Actual</t>
+  </si>
+  <si>
+    <t>Ont Senior Community Grant</t>
   </si>
 </sst>
 </file>
@@ -1940,8 +1940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3665FC8-9630-434E-9040-903A45656577}">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:K1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1975,7 +1975,7 @@
     </row>
     <row r="2" spans="1:11" ht="18.5">
       <c r="A2" s="142" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B2" s="143"/>
       <c r="C2" s="143"/>
@@ -2425,7 +2425,7 @@
         <v>0</v>
       </c>
       <c r="G16" s="53" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H16" s="91"/>
       <c r="I16" s="103">
@@ -2591,7 +2591,7 @@
       <c r="G21" s="56"/>
       <c r="H21" s="120" t="str">
         <f>Expenditure!B117</f>
-        <v>New Horizons for Seniors Program</v>
+        <v>Ont Senior Community Grant</v>
       </c>
       <c r="I21" s="105">
         <f>Expenditure!$E$117</f>
@@ -2714,7 +2714,7 @@
         <v>0</v>
       </c>
       <c r="G25" s="57" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H25" s="92"/>
       <c r="I25" s="103">
@@ -2734,7 +2734,7 @@
       <c r="A26" s="50"/>
       <c r="B26" s="78" t="str">
         <f>Offering!B26</f>
-        <v>New Horizons for Seniors Program</v>
+        <v>Ont Senior Community Grant</v>
       </c>
       <c r="C26" s="97">
         <f>Offering!$E$26</f>
@@ -2800,7 +2800,7 @@
     </row>
     <row r="29" spans="1:11">
       <c r="A29" s="128" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B29" s="129"/>
       <c r="C29" s="95">
@@ -2895,7 +2895,7 @@
     </row>
     <row r="34" spans="1:11">
       <c r="A34" s="130" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B34" s="131"/>
       <c r="C34" s="99">
@@ -2911,7 +2911,7 @@
         <v>0</v>
       </c>
       <c r="G34" s="140" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H34" s="141"/>
       <c r="I34" s="107">
@@ -2970,11 +2970,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E0CF550-27FC-43F1-88DC-1E797AD2F4C1}">
   <dimension ref="A1:S39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="5" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="E32" sqref="E32"/>
+      <selection pane="bottomRight" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2999,7 +2999,7 @@
     </row>
     <row r="2" spans="1:19" ht="15.5">
       <c r="A2" s="158" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B2" s="159"/>
       <c r="C2" s="159"/>
@@ -3036,19 +3036,19 @@
       </c>
       <c r="B5" s="162"/>
       <c r="C5" s="111" t="s">
+        <v>246</v>
+      </c>
+      <c r="D5" s="112" t="s">
         <v>247</v>
       </c>
-      <c r="D5" s="112" t="s">
-        <v>248</v>
-      </c>
       <c r="E5" s="113" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F5" s="62" t="s">
         <v>3</v>
       </c>
       <c r="G5" s="114" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H5" s="14" t="s">
         <v>174</v>
@@ -3661,7 +3661,7 @@
     <row r="26" spans="1:19">
       <c r="A26" s="12"/>
       <c r="B26" s="78" t="s">
-        <v>239</v>
+        <v>252</v>
       </c>
       <c r="C26" s="122">
         <v>21000</v>
@@ -3684,7 +3684,7 @@
     <row r="27" spans="1:19">
       <c r="A27" s="85"/>
       <c r="B27" s="78" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C27" s="122">
         <v>5000</v>
@@ -4050,10 +4050,10 @@
   <dimension ref="A1:S157"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C101" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C105" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="E108" sqref="E108"/>
+      <selection pane="bottomRight" activeCell="B118" sqref="B118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -4143,19 +4143,19 @@
         <v>2</v>
       </c>
       <c r="C4" s="115" t="s">
+        <v>246</v>
+      </c>
+      <c r="D4" s="116" t="s">
         <v>247</v>
       </c>
-      <c r="D4" s="116" t="s">
-        <v>248</v>
-      </c>
       <c r="E4" s="115" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F4" s="24" t="s">
         <v>3</v>
       </c>
       <c r="G4" s="116" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H4" s="16" t="s">
         <v>174</v>
@@ -8310,7 +8310,7 @@
         <v>160</v>
       </c>
       <c r="B117" s="118" t="s">
-        <v>239</v>
+        <v>252</v>
       </c>
       <c r="C117" s="75">
         <v>21000</v>
@@ -8341,10 +8341,10 @@
     </row>
     <row r="118" spans="1:19" s="76" customFormat="1" ht="14.5">
       <c r="A118" s="79" t="s">
+        <v>239</v>
+      </c>
+      <c r="B118" s="118" t="s">
         <v>240</v>
-      </c>
-      <c r="B118" s="118" t="s">
-        <v>241</v>
       </c>
       <c r="C118" s="75">
         <v>5000</v>
@@ -8938,7 +8938,7 @@
     <row r="7" spans="1:4">
       <c r="B7" t="str">
         <f>Summary!$B$26</f>
-        <v>New Horizons for Seniors Program</v>
+        <v>Ont Senior Community Grant</v>
       </c>
       <c r="C7" s="69">
         <f>Summary!$E$26</f>

</xml_diff>